<commit_message>
- changed id to ID - FFQSGRUREDMEAT Label ergänzt - hard cheese label ergänzt - changed label to alcopops instead of aperitif - added categories for variable K_FB_rauchkind_15
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_LISA_P1.xlsx
+++ b/rmonize/data_dictionary/DD_LISA_P1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EB6660-0962-49D3-8295-7C0B6F3267A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{30B8857A-D1A5-43D7-9D93-F1F7668B42E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
@@ -21,12 +21,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="219">
   <si>
     <t>index</t>
   </si>
@@ -40,7 +51,7 @@
     <t>valueType</t>
   </si>
   <si>
-    <t>id</t>
+    <t>ID</t>
   </si>
   <si>
     <t>ID of the participant</t>
@@ -64,9 +75,18 @@
     <t>Age at completion of 15-year questionnaire [years]</t>
   </si>
   <si>
+    <t>MUTBILD_0</t>
+  </si>
+  <si>
     <t>highest education of the mother</t>
   </si>
   <si>
+    <t>VATBILD_0</t>
+  </si>
+  <si>
+    <t>highest education of the father</t>
+  </si>
+  <si>
     <t>aktivleiisommn_15</t>
   </si>
   <si>
@@ -91,6 +111,9 @@
     <t>aktivmitwintn_15</t>
   </si>
   <si>
+    <t>Number of hours in a normal week (7 days) with moderate physical activity (some sweating, slightly increased breathing e.g. cycling, swimming, skating) in winter [hours]</t>
+  </si>
+  <si>
     <t>aktivschsommn_15</t>
   </si>
   <si>
@@ -112,7 +135,7 @@
     <t>UB_bmi_15</t>
   </si>
   <si>
-    <t>BMI bei 15-Jahresuntersuchung</t>
+    <t>measured BMI</t>
   </si>
   <si>
     <t>FFQGCAL_15</t>
@@ -244,6 +267,9 @@
     <t>FFQHARTK_15</t>
   </si>
   <si>
+    <t>hard cheese in g/d</t>
+  </si>
+  <si>
     <t>FFQNUD_15</t>
   </si>
   <si>
@@ -307,6 +333,9 @@
     <t>FFQSGRUREDMEAT_15</t>
   </si>
   <si>
+    <t>Total meat intake in g/d</t>
+  </si>
+  <si>
     <t>FFQHUHN_15</t>
   </si>
   <si>
@@ -481,12 +510,21 @@
     <t>ice cream in g/d</t>
   </si>
   <si>
+    <t>FFQKEKS_15</t>
+  </si>
+  <si>
     <t>biscuits in g/d</t>
   </si>
   <si>
+    <t>FFQOBSTK_15</t>
+  </si>
+  <si>
     <t>fruit cake in g/d</t>
   </si>
   <si>
+    <t>FFQTORTE_15</t>
+  </si>
+  <si>
     <t>cream cake in g/d</t>
   </si>
   <si>
@@ -496,6 +534,9 @@
     <t>Pastry in g/d</t>
   </si>
   <si>
+    <t>FFQRUEHRK_15</t>
+  </si>
+  <si>
     <t>sponge cake in g/d</t>
   </si>
   <si>
@@ -547,9 +588,21 @@
     <t>tea intake in g/d</t>
   </si>
   <si>
+    <t>K_FB_alkgetr_15</t>
+  </si>
+  <si>
+    <t>Total intake of alcoholic drinks, ml/d - 15y</t>
+  </si>
+  <si>
+    <t>K_FB_alkgetr_bier_15</t>
+  </si>
+  <si>
     <t>Intake of beer in ml/d</t>
   </si>
   <si>
+    <t>K_FB_alkgetr_wein_15</t>
+  </si>
+  <si>
     <t>Intake of wine in ml/d</t>
   </si>
   <si>
@@ -568,7 +621,7 @@
     <t>K_FB_alkgetr_alkopops_15</t>
   </si>
   <si>
-    <t>Intake of Aperitif (average Prosecco, Mix, Schnaps) in ml/d</t>
+    <t>Intake of alcopops in ml/d</t>
   </si>
   <si>
     <t>FFQCHIP_15</t>
@@ -586,9 +639,6 @@
     <t>female</t>
   </si>
   <si>
-    <t>MUTBILD_0</t>
-  </si>
-  <si>
     <t>No secondary school or elementary school certificate (Mother)</t>
   </si>
   <si>
@@ -610,45 +660,50 @@
     <t>Other degree (Mother)</t>
   </si>
   <si>
-    <t>TO BE COMPLETED</t>
-  </si>
-  <si>
-    <t>Number of hours in a normal week (7 days) with moderate physical activity (some sweating, slightly increased breathing e.g. cycling, swimming, skating) in winter [hours]</t>
-  </si>
-  <si>
-    <t>FFQKEKS_15</t>
-  </si>
-  <si>
-    <t>FFQOBSTK_15</t>
-  </si>
-  <si>
-    <t>FFQTORTE_15</t>
-  </si>
-  <si>
-    <t>FFQRUEHRK_15</t>
-  </si>
-  <si>
-    <t>K_FB_alkgetr_bier_15</t>
-  </si>
-  <si>
-    <t>K_FB_alkgetr_wein_15</t>
+    <t>No secondary school or elementary school certificate</t>
+  </si>
+  <si>
+    <t>Lower secondary school or elementary school certificate</t>
+  </si>
+  <si>
+    <t>Secondary school certificate (middle school leaving certificate)</t>
+  </si>
+  <si>
+    <t>Completion of Polytechnic. high school</t>
+  </si>
+  <si>
+    <t>Advanced technical college entrance qualification</t>
+  </si>
+  <si>
+    <t>general or specialist university entrance qualification</t>
+  </si>
+  <si>
+    <t>other degree</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes, daily</t>
+  </si>
+  <si>
+    <t>yes, several times a week</t>
+  </si>
+  <si>
+    <t>yes, once a week</t>
+  </si>
+  <si>
+    <t>yes, less often</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -666,6 +721,25 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -688,30 +762,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -727,7 +820,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1023,13 +1116,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="3"/>
     <col min="2" max="2" width="26.28515625" style="5" customWidth="1"/>
@@ -1098,10 +1191,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -1112,13 +1205,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" s="7" t="s">
         <v>15</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1132,7 +1225,7 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1140,13 +1233,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1154,13 +1247,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>195</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1168,13 +1261,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1182,13 +1275,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1196,13 +1289,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1210,13 +1303,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1224,13 +1317,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1238,13 +1331,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1252,13 +1345,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1266,13 +1359,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1280,13 +1373,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1294,13 +1387,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1308,13 +1401,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1322,13 +1415,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1336,13 +1429,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1350,13 +1443,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1364,13 +1457,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1378,13 +1471,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1392,13 +1485,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D26" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1406,13 +1499,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1420,13 +1513,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1434,13 +1527,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D29" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1448,13 +1541,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D30" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1462,13 +1555,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D31" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1476,13 +1569,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D32" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1490,13 +1583,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D33" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1504,13 +1597,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D34" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1518,13 +1611,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C35" t="s">
-        <v>194</v>
+        <v>74</v>
       </c>
       <c r="D35" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1532,13 +1625,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D36" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1546,13 +1639,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D37" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1560,13 +1653,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D38" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1574,13 +1667,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D39" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1588,13 +1681,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C40" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D40" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1602,13 +1695,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D41" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1616,13 +1709,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D42" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1630,13 +1723,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C43" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D43" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1644,13 +1737,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D44" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1658,13 +1751,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C45" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D45" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1672,13 +1765,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C46" t="s">
-        <v>194</v>
+        <v>96</v>
       </c>
       <c r="D46" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1686,13 +1779,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C47" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D47" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1700,13 +1793,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C48" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D48" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1714,13 +1807,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C49" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D49" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1728,13 +1821,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C50" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D50" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1742,13 +1835,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C51" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D51" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1756,13 +1849,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C52" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D52" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1770,13 +1863,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C53" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D53" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1784,13 +1877,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C54" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D54" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1798,13 +1891,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C55" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D55" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1812,13 +1905,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C56" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D56" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1826,13 +1919,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C57" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D57" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1840,13 +1933,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C58" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D58" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1854,13 +1947,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C59" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D59" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1868,13 +1961,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C60" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D60" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1882,13 +1975,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C61" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D61" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1896,13 +1989,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C62" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D62" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1910,13 +2003,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C63" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D63" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1924,13 +2017,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C64" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D64" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1938,13 +2031,13 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C65" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D65" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1952,13 +2045,13 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C66" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D66" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1966,13 +2059,13 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C67" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D67" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1980,13 +2073,13 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C68" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D68" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1994,13 +2087,13 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C69" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2008,13 +2101,13 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C70" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D70" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2022,13 +2115,13 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C71" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D71" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2036,13 +2129,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C72" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D72" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2050,13 +2143,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C73" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D73" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2064,13 +2157,13 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C74" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D74" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2078,13 +2171,13 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C75" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D75" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2092,13 +2185,13 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>196</v>
+        <v>155</v>
       </c>
       <c r="C76" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="D76" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2106,13 +2199,13 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>197</v>
+        <v>157</v>
       </c>
       <c r="C77" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="D77" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2120,13 +2213,13 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>198</v>
+        <v>159</v>
       </c>
       <c r="C78" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D78" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2134,13 +2227,13 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="C79" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="D79" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2148,13 +2241,13 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>199</v>
+        <v>163</v>
       </c>
       <c r="C80" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D80" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2162,13 +2255,13 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C81" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="D81" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2176,13 +2269,13 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="C82" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="D82" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2190,13 +2283,13 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="C83" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="D83" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2204,13 +2297,13 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="C84" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="D84" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2218,13 +2311,13 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="C85" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="D85" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2232,13 +2325,13 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="C86" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="D86" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2246,13 +2339,13 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C87" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="D87" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2260,13 +2353,13 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="C88" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D88" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2274,27 +2367,27 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="C89" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="D89" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
-      <c r="B90" t="s">
-        <v>201</v>
+      <c r="B90" s="12" t="s">
+        <v>183</v>
       </c>
       <c r="C90" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="D90" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2302,13 +2395,13 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="C91" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="D91" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2316,13 +2409,13 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="C92" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="D92" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2330,13 +2423,13 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>179</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>180</v>
+        <v>189</v>
+      </c>
+      <c r="C93" t="s">
+        <v>190</v>
       </c>
       <c r="D93" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2344,13 +2437,41 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="C94" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="D94" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>193</v>
+      </c>
+      <c r="C95" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D95" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>195</v>
+      </c>
+      <c r="C96" t="s">
+        <v>196</v>
+      </c>
+      <c r="D96" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2361,13 +2482,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CFBFAA-22DC-428C-A718-7E0BADD40216}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="3"/>
@@ -2376,7 +2497,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2394,7 +2515,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2405,84 +2526,216 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>186</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>186</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>186</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>186</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3">
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>186</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3">
         <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>186</v>
+        <v>12</v>
       </c>
       <c r="B9" s="3">
         <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>186</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3">
         <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>193</v>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="11">
+        <v>2</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="11">
+        <v>3</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="11">
+        <v>4</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="11">
+        <v>5</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="11">
+        <v>6</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="11">
+        <v>7</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="11">
+        <v>2</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="11">
+        <v>3</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="11">
+        <v>4</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="11">
+        <v>5</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2763,13 +3016,13 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -2778,7 +3031,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{607F74A7-32EE-406C-A688-0D84C4E12BE8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E15759D-0549-4559-B749-E28DD96246FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>

</xml_diff>

<commit_message>
GL-4 DD_LISA_P1 small update to match P2
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_LISA_P1.xlsx
+++ b/rmonize/data_dictionary/DD_LISA_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30B8857A-D1A5-43D7-9D93-F1F7668B42E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE44F3B-8BED-40B1-A352-D418CC600C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11025" windowHeight="11760" activeTab="1" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -26,10 +26,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="214">
   <si>
     <t>index</t>
   </si>
@@ -639,27 +639,6 @@
     <t>female</t>
   </si>
   <si>
-    <t>No secondary school or elementary school certificate (Mother)</t>
-  </si>
-  <si>
-    <t>Lower secondary school or elementary school certificate (Mother)</t>
-  </si>
-  <si>
-    <t>Secondary school certificate (middle school leaving certificate)(Mother)</t>
-  </si>
-  <si>
-    <t>Completion of Polytechnic. high school (Mother)</t>
-  </si>
-  <si>
-    <t>Advanced technical college entrance qualification (Mother)</t>
-  </si>
-  <si>
-    <t>General or specialist university entrance qualification (Mother)</t>
-  </si>
-  <si>
-    <t>Other degree (Mother)</t>
-  </si>
-  <si>
     <t>No secondary school or elementary school certificate</t>
   </si>
   <si>
@@ -694,6 +673,12 @@
   </si>
   <si>
     <t>yes, less often</t>
+  </si>
+  <si>
+    <t>Other degree</t>
+  </si>
+  <si>
+    <t>General or specialist university entrance qualification</t>
   </si>
 </sst>
 </file>
@@ -804,7 +789,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -820,9 +805,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -860,7 +845,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -966,7 +951,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1108,7 +1093,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1118,11 +1103,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
   <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="3"/>
     <col min="2" max="2" width="26.28515625" style="5" customWidth="1"/>
@@ -2484,11 +2469,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CFBFAA-22DC-428C-A718-7E0BADD40216}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="3"/>
@@ -2529,7 +2514,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
@@ -2540,7 +2525,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
@@ -2592,7 +2577,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2603,7 +2588,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2614,7 +2599,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2625,7 +2610,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2636,7 +2621,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2647,7 +2632,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2658,7 +2643,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2669,7 +2654,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2680,7 +2665,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2691,7 +2676,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2702,7 +2687,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2713,7 +2698,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2724,7 +2709,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2735,7 +2720,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2744,15 +2729,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -2762,6 +2738,15 @@
     <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3006,14 +2991,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3026,6 +3003,14 @@
     <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>